<commit_message>
Exceptions are added to depot form. Code documentation is added too.
</commit_message>
<xml_diff>
--- a/Architecture/bin/Debug/ProductData.xlsx
+++ b/Architecture/bin/Debug/ProductData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>RequestID</t>
   </si>
@@ -94,24 +94,12 @@
     <t>20/03/2020</t>
   </si>
   <si>
-    <t>Galaxy A40</t>
+    <t>Galaxy A30</t>
   </si>
   <si>
     <t>Smart Phone</t>
   </si>
   <si>
-    <t>Marketing</t>
-  </si>
-  <si>
-    <t>13/05/2020</t>
-  </si>
-  <si>
-    <t>15/05/2020</t>
-  </si>
-  <si>
-    <t>Galaxy A30</t>
-  </si>
-  <si>
     <t>Service</t>
   </si>
   <si>
@@ -119,6 +107,12 @@
   </si>
   <si>
     <t>17/06/2020</t>
+  </si>
+  <si>
+    <t>ES1-572</t>
+  </si>
+  <si>
+    <t>19/06/2020</t>
   </si>
 </sst>
 </file>
@@ -682,7 +676,7 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>1254</v>
+        <v>1283</v>
       </c>
       <c r="B9" t="s">
         <v>26</v>
@@ -697,7 +691,7 @@
         <v>28</v>
       </c>
       <c r="F9">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
         <v>29</v>
@@ -708,28 +702,28 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>1283</v>
+        <v>1287</v>
       </c>
       <c r="B10" t="s">
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" t="s">
         <v>32</v>
-      </c>
-      <c r="F10">
-        <v>12</v>
-      </c>
-      <c r="G10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>